<commit_message>
feat(gui): add Excel data viewing and saving functionality
- Implement loading Excel data into QTableWidget
- Add saving QTableWidget data to Excel file
- Implement Ctrl+S shortcut for saving table data
- Create separate check_window.py for Excel viewing
- Update main_window to open check_window via button click
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_manual_input_data.xlsx
+++ b/src/data/input/manual/temp_manual_input_data.xlsx
@@ -488,32 +488,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>1231</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>23123</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>123</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>12312</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>3123</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>1231</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(gui): resolve circular import and improve QLineEdit reset
- Rename ui_utils.py to detail_ui_button_utils.py to avoid circular import
- Implement lazy importing to break the circular dependency
- Add data_save_success function for saving confirmation dialog
- Update QLineEdit reset method to use setText() instead of direct assignment
- Improve code structure and add comments for better understanding
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_manual_input_data.xlsx
+++ b/src/data/input/manual/temp_manual_input_data.xlsx
@@ -478,42 +478,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-04-27</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1231</t>
+          <t>12</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>23123</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>12312</t>
+          <t>12</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3123</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1231</t>
+          <t>12</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(gui): implement temporary storage and update stored item count
- Add temporary storage functionality for single entry form
- Update stored item count display after each successful storage
- Refactor UI layout and improve element naming
- Implement main module variable access and update from utils module
- Optimize TODO list and documentation for better code structure and maintenance
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_manual_input_data.xlsx
+++ b/src/data/input/manual/temp_manual_input_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,46 +474,56 @@
           <t>单位</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>公司</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(gui): implement temp data storage and rollback functionality
- Add temp data storage to Excel file
- Implement window closure to clear temp storage
- Add spinbox control for navigation between stored items
- Implement rollback functionality for stored items
- Update stored item count dynamically
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_manual_input_data.xlsx
+++ b/src/data/input/manual/temp_manual_input_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,53 +480,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix(gui): resolve index out of range error and improve excel data commit flow
- Add IndexOutOfRange class to handle index out of range error
- Update temp_list_rollback function to handle different index input scenarios
- Implement commit_data_to_excel function to submit data to Excel
- Fix circular import error in ui_utils.py
- Update error handling and user interface for better error messaging
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_manual_input_data.xlsx
+++ b/src/data/input/manual/temp_manual_input_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +480,53 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-05-01</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1212</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(core): implement data commit functionality from temp to main Excel
- Add `cmmit_data_to_storage_excel` function in excel_handler.py to commit data from temp Excel to main/sub Excel files
- Update `store_single_entry_to_temple_excel` to reflect the new function name
- Modify `commit_data_to_excel` in detail_ui_button_utils.py to use the new commit function
- Add main and sub Excel file paths in main_window.py
- Connect commit button to commit function in UI setup
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_manual_input_data.xlsx
+++ b/src/data/input/manual/temp_manual_input_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,53 +480,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-05-01</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>1212</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: update compiled Python files and Excel input template
- Update compiled Python files for excel_handler, check_window, data_save_dialog, error_window, main_window, and detail_ui_button_utils
- Update temp_manual_input_data.xlsx file in the input/manual directory
</commit_message>
<xml_diff>
--- a/src/data/input/manual/temp_manual_input_data.xlsx
+++ b/src/data/input/manual/temp_manual_input_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -478,37 +478,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>2025-04-29</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>12</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>12</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>21</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">

</xml_diff>